<commit_message>
Changes added to three marker problems
</commit_message>
<xml_diff>
--- a/HealthPath/CreatingReport/Encyclopedia_mod with ranges_PN20190822.xlsx
+++ b/HealthPath/CreatingReport/Encyclopedia_mod with ranges_PN20190822.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="767" uniqueCount="532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="533">
   <si>
     <t xml:space="preserve">Code</t>
   </si>
@@ -1546,13 +1546,13 @@
     <t xml:space="preserve">We have discovered 17 different types of Blastocystis so far, and not all of them cause symptoms. The faecal-to-oral route is the most common mode of infection, which means we typically get it through drinking contaminated water or through poor hygiene practices.</t>
   </si>
   <si>
+    <t xml:space="preserve">Borderline</t>
+  </si>
+  <si>
     <t xml:space="preserve">A parasite that may or may not cause symptoms. Unfriendly.</t>
   </si>
   <si>
     <t xml:space="preserve">Infection by Blastocystis hominis can show up as diarrhoea, abdominal pain, fatigue, constipation, flatulence, IBS or skin conditions.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Borderline</t>
   </si>
   <si>
     <t xml:space="preserve">DIENTAMOEBFA178</t>
@@ -1920,6 +1920,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">HBFE</t>
+  </si>
+  <si>
     <t xml:space="preserve">Haemoglobin in faeces</t>
   </si>
   <si>
@@ -2097,7 +2100,7 @@
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2213,6 +2216,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i val="true"/>
@@ -2425,7 +2433,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="101">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2750,6 +2758,10 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2766,11 +2778,11 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2782,47 +2794,47 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="21" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="22" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="10" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="21" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="21" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="11" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2905,8 +2917,8 @@
   </sheetPr>
   <dimension ref="A1:M303"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A241" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A243" activeCellId="0" sqref="A243"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D292" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M187" activeCellId="0" sqref="M187"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5910,6 +5922,7 @@
       </c>
       <c r="K161" s="17"/>
       <c r="L161" s="17"/>
+      <c r="M161" s="0"/>
     </row>
     <row r="162" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B162" s="30" t="s">
@@ -6382,6 +6395,7 @@
         <v>333</v>
       </c>
       <c r="L187" s="17"/>
+      <c r="M187" s="0"/>
     </row>
     <row r="188" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B188" s="30" t="s">
@@ -6520,8 +6534,8 @@
       <c r="K195" s="17"/>
       <c r="L195" s="17"/>
     </row>
-    <row r="196" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A196" s="13" t="s">
+    <row r="196" customFormat="false" ht="33.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A196" s="81" t="s">
         <v>343</v>
       </c>
       <c r="B196" s="27" t="s">
@@ -6981,16 +6995,20 @@
       <c r="B221" s="27" t="s">
         <v>378</v>
       </c>
-      <c r="C221" s="81" t="s">
+      <c r="C221" s="82" t="s">
         <v>379</v>
       </c>
       <c r="D221" s="55"/>
       <c r="E221" s="17"/>
       <c r="F221" s="17"/>
       <c r="G221" s="17"/>
-      <c r="H221" s="17"/>
+      <c r="H221" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="I221" s="17"/>
-      <c r="J221" s="17"/>
+      <c r="J221" s="17" t="s">
+        <v>101</v>
+      </c>
       <c r="K221" s="17"/>
       <c r="L221" s="17"/>
     </row>
@@ -6998,18 +7016,14 @@
       <c r="B222" s="40" t="s">
         <v>380</v>
       </c>
-      <c r="C222" s="81"/>
+      <c r="C222" s="82"/>
       <c r="D222" s="55"/>
       <c r="E222" s="17"/>
       <c r="F222" s="17"/>
       <c r="G222" s="17"/>
-      <c r="H222" s="17" t="s">
-        <v>100</v>
-      </c>
+      <c r="H222" s="17"/>
       <c r="I222" s="17"/>
-      <c r="J222" s="17" t="s">
-        <v>101</v>
-      </c>
+      <c r="J222" s="17"/>
       <c r="K222" s="17"/>
       <c r="L222" s="17"/>
     </row>
@@ -7043,7 +7057,7 @@
       <c r="K224" s="17"/>
       <c r="L224" s="17"/>
     </row>
-    <row r="225" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="225" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A225" s="13" t="s">
         <v>383</v>
       </c>
@@ -7057,15 +7071,21 @@
       <c r="E225" s="17"/>
       <c r="F225" s="17"/>
       <c r="G225" s="17"/>
-      <c r="H225" s="17"/>
-      <c r="I225" s="17"/>
-      <c r="J225" s="17"/>
+      <c r="H225" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="I225" s="17" t="s">
+        <v>386</v>
+      </c>
+      <c r="J225" s="17" t="s">
+        <v>101</v>
+      </c>
       <c r="K225" s="17"/>
       <c r="L225" s="17"/>
     </row>
     <row r="226" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B226" s="30" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C226" s="28"/>
       <c r="D226" s="55"/>
@@ -7081,25 +7101,19 @@
     <row r="227" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B227" s="31"/>
       <c r="C227" s="34" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="D227" s="55"/>
       <c r="E227" s="17"/>
       <c r="F227" s="17"/>
       <c r="G227" s="17"/>
-      <c r="H227" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="I227" s="17" t="s">
-        <v>388</v>
-      </c>
-      <c r="J227" s="17" t="s">
-        <v>101</v>
-      </c>
+      <c r="H227" s="17"/>
+      <c r="I227" s="17"/>
+      <c r="J227" s="17"/>
       <c r="K227" s="17"/>
       <c r="L227" s="17"/>
     </row>
-    <row r="228" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="228" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A228" s="13" t="s">
         <v>389</v>
       </c>
@@ -7113,9 +7127,15 @@
       <c r="E228" s="17"/>
       <c r="F228" s="17"/>
       <c r="G228" s="17"/>
-      <c r="H228" s="17"/>
-      <c r="I228" s="17"/>
-      <c r="J228" s="17"/>
+      <c r="H228" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="I228" s="17" t="s">
+        <v>386</v>
+      </c>
+      <c r="J228" s="17" t="s">
+        <v>101</v>
+      </c>
       <c r="K228" s="17"/>
       <c r="L228" s="17"/>
     </row>
@@ -7143,15 +7163,9 @@
       <c r="E230" s="17"/>
       <c r="F230" s="17"/>
       <c r="G230" s="17"/>
-      <c r="H230" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="I230" s="17" t="s">
-        <v>388</v>
-      </c>
-      <c r="J230" s="17" t="s">
-        <v>101</v>
-      </c>
+      <c r="H230" s="17"/>
+      <c r="I230" s="17"/>
+      <c r="J230" s="17"/>
       <c r="K230" s="17"/>
       <c r="L230" s="17"/>
     </row>
@@ -7169,9 +7183,13 @@
       <c r="E231" s="22"/>
       <c r="F231" s="22"/>
       <c r="G231" s="22"/>
-      <c r="H231" s="22"/>
+      <c r="H231" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="I231" s="22"/>
-      <c r="J231" s="22"/>
+      <c r="J231" s="17" t="s">
+        <v>101</v>
+      </c>
       <c r="K231" s="22"/>
       <c r="L231" s="22"/>
       <c r="M231" s="50"/>
@@ -7221,7 +7239,7 @@
       <c r="K234" s="17"/>
       <c r="L234" s="17"/>
     </row>
-    <row r="235" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="235" customFormat="false" ht="82.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A235" s="13" t="s">
         <v>400</v>
       </c>
@@ -7235,9 +7253,13 @@
       <c r="E235" s="17"/>
       <c r="F235" s="17"/>
       <c r="G235" s="17"/>
-      <c r="H235" s="17"/>
+      <c r="H235" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="I235" s="17"/>
-      <c r="J235" s="17"/>
+      <c r="J235" s="17" t="s">
+        <v>101</v>
+      </c>
       <c r="K235" s="17"/>
       <c r="L235" s="17"/>
     </row>
@@ -7265,17 +7287,13 @@
       <c r="E237" s="17"/>
       <c r="F237" s="17"/>
       <c r="G237" s="17"/>
-      <c r="H237" s="17" t="s">
-        <v>100</v>
-      </c>
+      <c r="H237" s="17"/>
       <c r="I237" s="17"/>
-      <c r="J237" s="17" t="s">
-        <v>101</v>
-      </c>
+      <c r="J237" s="17"/>
       <c r="K237" s="17"/>
       <c r="L237" s="17"/>
     </row>
-    <row r="238" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="238" customFormat="false" ht="59.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A238" s="13" t="s">
         <v>405</v>
       </c>
@@ -7289,9 +7307,13 @@
       <c r="E238" s="17"/>
       <c r="F238" s="17"/>
       <c r="G238" s="17"/>
-      <c r="H238" s="17"/>
+      <c r="H238" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="I238" s="17"/>
-      <c r="J238" s="17"/>
+      <c r="J238" s="17" t="s">
+        <v>101</v>
+      </c>
       <c r="K238" s="17"/>
       <c r="L238" s="17"/>
     </row>
@@ -7319,17 +7341,13 @@
       <c r="E240" s="17"/>
       <c r="F240" s="17"/>
       <c r="G240" s="17"/>
-      <c r="H240" s="17" t="s">
-        <v>100</v>
-      </c>
+      <c r="H240" s="17"/>
       <c r="I240" s="17"/>
-      <c r="J240" s="17" t="s">
-        <v>101</v>
-      </c>
+      <c r="J240" s="17"/>
       <c r="K240" s="17"/>
       <c r="L240" s="17"/>
     </row>
-    <row r="241" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="241" customFormat="false" ht="48.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A241" s="13" t="s">
         <v>410</v>
       </c>
@@ -7343,9 +7361,13 @@
       <c r="E241" s="17"/>
       <c r="F241" s="17"/>
       <c r="G241" s="17"/>
-      <c r="H241" s="17"/>
+      <c r="H241" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="I241" s="17"/>
-      <c r="J241" s="17"/>
+      <c r="J241" s="17" t="s">
+        <v>101</v>
+      </c>
       <c r="K241" s="17"/>
       <c r="L241" s="17"/>
     </row>
@@ -7373,17 +7395,13 @@
       <c r="E243" s="17"/>
       <c r="F243" s="17"/>
       <c r="G243" s="17"/>
-      <c r="H243" s="17" t="s">
-        <v>100</v>
-      </c>
+      <c r="H243" s="17"/>
       <c r="I243" s="17"/>
-      <c r="J243" s="17" t="s">
-        <v>101</v>
-      </c>
+      <c r="J243" s="17"/>
       <c r="K243" s="17"/>
       <c r="L243" s="17"/>
     </row>
-    <row r="244" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="244" customFormat="false" ht="36.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A244" s="13" t="s">
         <v>415</v>
       </c>
@@ -7397,9 +7415,13 @@
       <c r="E244" s="17"/>
       <c r="F244" s="17"/>
       <c r="G244" s="17"/>
-      <c r="H244" s="17"/>
+      <c r="H244" s="17" t="s">
+        <v>100</v>
+      </c>
       <c r="I244" s="17"/>
-      <c r="J244" s="17"/>
+      <c r="J244" s="17" t="s">
+        <v>101</v>
+      </c>
       <c r="K244" s="17"/>
       <c r="L244" s="17"/>
     </row>
@@ -7427,13 +7449,9 @@
       <c r="E246" s="17"/>
       <c r="F246" s="17"/>
       <c r="G246" s="17"/>
-      <c r="H246" s="17" t="s">
-        <v>100</v>
-      </c>
+      <c r="H246" s="17"/>
       <c r="I246" s="17"/>
-      <c r="J246" s="17" t="s">
-        <v>101</v>
-      </c>
+      <c r="J246" s="17"/>
       <c r="K246" s="17"/>
       <c r="L246" s="17"/>
     </row>
@@ -7520,25 +7538,21 @@
       <c r="B252" s="48" t="s">
         <v>426</v>
       </c>
-      <c r="C252" s="82" t="s">
+      <c r="C252" s="83" t="s">
         <v>427</v>
       </c>
       <c r="D252" s="80"/>
       <c r="E252" s="22"/>
       <c r="F252" s="22"/>
       <c r="G252" s="22"/>
-      <c r="H252" s="22" t="s">
-        <v>100</v>
-      </c>
+      <c r="H252" s="22"/>
       <c r="I252" s="22"/>
-      <c r="J252" s="22" t="s">
-        <v>101</v>
-      </c>
+      <c r="J252" s="22"/>
       <c r="K252" s="22"/>
       <c r="L252" s="22"/>
       <c r="M252" s="50"/>
     </row>
-    <row r="253" s="47" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="253" s="47" customFormat="true" ht="89.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B253" s="78" t="s">
         <v>428</v>
       </c>
@@ -7549,9 +7563,13 @@
       <c r="E253" s="22"/>
       <c r="F253" s="22"/>
       <c r="G253" s="22"/>
-      <c r="H253" s="22"/>
+      <c r="H253" s="22" t="s">
+        <v>100</v>
+      </c>
       <c r="I253" s="22"/>
-      <c r="J253" s="22"/>
+      <c r="J253" s="22" t="s">
+        <v>101</v>
+      </c>
       <c r="K253" s="22"/>
       <c r="L253" s="22"/>
       <c r="M253" s="50"/>
@@ -7679,7 +7697,7 @@
       <c r="B261" s="48" t="s">
         <v>439</v>
       </c>
-      <c r="C261" s="83" t="s">
+      <c r="C261" s="84" t="s">
         <v>440</v>
       </c>
       <c r="D261" s="80"/>
@@ -7734,7 +7752,7 @@
       <c r="B264" s="48" t="s">
         <v>444</v>
       </c>
-      <c r="C264" s="84" t="s">
+      <c r="C264" s="85" t="s">
         <v>445</v>
       </c>
       <c r="D264" s="80"/>
@@ -7908,7 +7926,7 @@
       <c r="B274" s="48" t="s">
         <v>458</v>
       </c>
-      <c r="C274" s="82" t="s">
+      <c r="C274" s="83" t="s">
         <v>459</v>
       </c>
       <c r="D274" s="80"/>
@@ -7963,7 +7981,7 @@
       <c r="B277" s="48" t="s">
         <v>463</v>
       </c>
-      <c r="C277" s="84" t="s">
+      <c r="C277" s="85" t="s">
         <v>464</v>
       </c>
       <c r="D277" s="80"/>
@@ -8066,7 +8084,7 @@
     </row>
     <row r="283" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B283" s="53"/>
-      <c r="C283" s="85" t="s">
+      <c r="C283" s="86" t="s">
         <v>473</v>
       </c>
       <c r="D283" s="80"/>
@@ -8081,7 +8099,7 @@
     </row>
     <row r="284" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B284" s="53"/>
-      <c r="C284" s="85" t="s">
+      <c r="C284" s="86" t="s">
         <v>474</v>
       </c>
       <c r="D284" s="80"/>
@@ -8096,7 +8114,7 @@
     </row>
     <row r="285" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B285" s="31"/>
-      <c r="C285" s="86" t="s">
+      <c r="C285" s="87" t="s">
         <v>475</v>
       </c>
       <c r="D285" s="80"/>
@@ -8110,18 +8128,21 @@
       <c r="L285" s="17"/>
     </row>
     <row r="286" s="47" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A286" s="47" t="s">
+        <v>476</v>
+      </c>
       <c r="B286" s="78" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C286" s="79" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="D286" s="80"/>
       <c r="E286" s="22"/>
       <c r="F286" s="22"/>
       <c r="G286" s="22"/>
       <c r="H286" s="22" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="I286" s="22"/>
       <c r="J286" s="22"/>
@@ -8131,7 +8152,7 @@
     </row>
     <row r="287" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B287" s="30" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C287" s="28"/>
       <c r="D287" s="80"/>
@@ -8147,7 +8168,7 @@
     <row r="288" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B288" s="31"/>
       <c r="C288" s="34" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="D288" s="80"/>
       <c r="E288" s="17"/>
@@ -8161,16 +8182,16 @@
     </row>
     <row r="289" s="47" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A289" s="26" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="B289" s="78" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="C289" s="79" t="s">
-        <v>483</v>
-      </c>
-      <c r="D289" s="87" t="s">
         <v>484</v>
+      </c>
+      <c r="D289" s="88" t="s">
+        <v>485</v>
       </c>
       <c r="E289" s="22" t="n">
         <v>0</v>
@@ -8182,7 +8203,7 @@
         <v>340</v>
       </c>
       <c r="H289" s="22" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="I289" s="22" t="n">
         <v>3040</v>
@@ -8194,11 +8215,11 @@
         <v>5040</v>
       </c>
       <c r="L289" s="22"/>
-      <c r="M289" s="50"/>
+      <c r="M289" s="0"/>
     </row>
     <row r="290" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B290" s="30" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C290" s="28"/>
       <c r="D290" s="29"/>
@@ -8214,10 +8235,10 @@
     <row r="291" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B291" s="53"/>
       <c r="C291" s="59" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D291" s="42" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="E291" s="17"/>
       <c r="F291" s="17"/>
@@ -8244,7 +8265,7 @@
     <row r="293" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B293" s="53"/>
       <c r="C293" s="28" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="D293" s="43"/>
       <c r="E293" s="17"/>
@@ -8271,14 +8292,14 @@
     </row>
     <row r="295" s="47" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A295" s="26" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B295" s="78" t="s">
-        <v>491</v>
-      </c>
-      <c r="C295" s="88"/>
-      <c r="D295" s="87" t="s">
         <v>492</v>
+      </c>
+      <c r="C295" s="89"/>
+      <c r="D295" s="88" t="s">
+        <v>493</v>
       </c>
       <c r="E295" s="22" t="n">
         <v>54</v>
@@ -8290,7 +8311,7 @@
         <v>199</v>
       </c>
       <c r="H295" s="22" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="I295" s="22"/>
       <c r="J295" s="22"/>
@@ -8300,9 +8321,9 @@
     </row>
     <row r="296" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B296" s="30" t="s">
-        <v>494</v>
-      </c>
-      <c r="C296" s="88"/>
+        <v>495</v>
+      </c>
+      <c r="C296" s="89"/>
       <c r="D296" s="42"/>
       <c r="E296" s="17"/>
       <c r="F296" s="17"/>
@@ -8315,9 +8336,9 @@
     </row>
     <row r="297" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B297" s="31"/>
-      <c r="C297" s="88"/>
+      <c r="C297" s="89"/>
       <c r="D297" s="33" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="E297" s="17"/>
       <c r="F297" s="17"/>
@@ -8330,20 +8351,20 @@
     </row>
     <row r="298" s="47" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A298" s="26" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B298" s="78" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C298" s="79" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="D298" s="80"/>
       <c r="E298" s="22"/>
       <c r="F298" s="22"/>
       <c r="G298" s="22"/>
       <c r="H298" s="22" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="I298" s="22" t="n">
         <v>75</v>
@@ -8357,7 +8378,7 @@
     </row>
     <row r="299" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B299" s="30" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C299" s="28"/>
       <c r="D299" s="80"/>
@@ -8373,7 +8394,7 @@
     <row r="300" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B300" s="31"/>
       <c r="C300" s="34" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="D300" s="80"/>
       <c r="E300" s="17"/>
@@ -8387,13 +8408,13 @@
     </row>
     <row r="301" s="47" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B301" s="78" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C301" s="79" t="s">
-        <v>503</v>
-      </c>
-      <c r="D301" s="87" t="s">
-        <v>503</v>
+        <v>504</v>
+      </c>
+      <c r="D301" s="88" t="s">
+        <v>504</v>
       </c>
       <c r="E301" s="22"/>
       <c r="F301" s="22"/>
@@ -8409,7 +8430,7 @@
     </row>
     <row r="302" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B302" s="30" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C302" s="28"/>
       <c r="D302" s="29"/>
@@ -8425,10 +8446,10 @@
     <row r="303" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B303" s="31"/>
       <c r="C303" s="34" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="D303" s="35" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="E303" s="17"/>
       <c r="F303" s="17"/>
@@ -8544,7 +8565,7 @@
   </sheetPr>
   <dimension ref="A3:N24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A29" activeCellId="0" sqref="A29"/>
     </sheetView>
   </sheetViews>
@@ -8559,438 +8580,438 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="42" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="89" t="s">
-        <v>507</v>
-      </c>
-      <c r="B4" s="90"/>
-      <c r="C4" s="90"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="90"/>
-      <c r="F4" s="90"/>
-      <c r="G4" s="90"/>
-      <c r="H4" s="90"/>
-      <c r="I4" s="90"/>
-      <c r="J4" s="90"/>
-      <c r="K4" s="90"/>
-      <c r="L4" s="90"/>
-      <c r="M4" s="90"/>
-      <c r="N4" s="90"/>
+      <c r="A4" s="90" t="s">
+        <v>508</v>
+      </c>
+      <c r="B4" s="91"/>
+      <c r="C4" s="91"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="91"/>
+      <c r="F4" s="91"/>
+      <c r="G4" s="91"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="91"/>
+      <c r="J4" s="91"/>
+      <c r="K4" s="91"/>
+      <c r="L4" s="91"/>
+      <c r="M4" s="91"/>
+      <c r="N4" s="91"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="89" t="s">
-        <v>508</v>
-      </c>
-      <c r="B5" s="91" t="s">
+      <c r="A5" s="90" t="s">
         <v>509</v>
       </c>
-      <c r="C5" s="89" t="s">
+      <c r="B5" s="92" t="s">
         <v>510</v>
       </c>
-      <c r="D5" s="91" t="s">
+      <c r="C5" s="90" t="s">
         <v>511</v>
       </c>
-      <c r="E5" s="91" t="s">
+      <c r="D5" s="92" t="s">
         <v>512</v>
       </c>
-      <c r="F5" s="91" t="s">
+      <c r="E5" s="92" t="s">
         <v>513</v>
       </c>
-      <c r="G5" s="91" t="s">
+      <c r="F5" s="92" t="s">
         <v>514</v>
       </c>
-      <c r="H5" s="91" t="s">
+      <c r="G5" s="92" t="s">
         <v>515</v>
       </c>
-      <c r="I5" s="91" t="s">
+      <c r="H5" s="92" t="s">
         <v>516</v>
       </c>
-      <c r="J5" s="91" t="s">
+      <c r="I5" s="92" t="s">
         <v>517</v>
       </c>
-      <c r="K5" s="91" t="s">
+      <c r="J5" s="92" t="s">
         <v>518</v>
       </c>
-      <c r="L5" s="91" t="s">
+      <c r="K5" s="92" t="s">
         <v>519</v>
       </c>
-      <c r="M5" s="91" t="s">
+      <c r="L5" s="92" t="s">
         <v>520</v>
       </c>
-      <c r="N5" s="89" t="s">
+      <c r="M5" s="92" t="s">
         <v>521</v>
       </c>
+      <c r="N5" s="90" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="92" t="s">
-        <v>522</v>
-      </c>
-      <c r="B6" s="93" t="n">
+      <c r="A6" s="93" t="s">
+        <v>523</v>
+      </c>
+      <c r="B6" s="94" t="n">
         <v>180</v>
       </c>
-      <c r="C6" s="92" t="s">
+      <c r="C6" s="93" t="s">
+        <v>524</v>
+      </c>
+      <c r="D6" s="95"/>
+      <c r="E6" s="95"/>
+      <c r="F6" s="95"/>
+      <c r="G6" s="95"/>
+      <c r="H6" s="95"/>
+      <c r="I6" s="94" t="n">
+        <v>280</v>
+      </c>
+      <c r="J6" s="94" t="n">
+        <v>330</v>
+      </c>
+      <c r="K6" s="95"/>
+      <c r="L6" s="95"/>
+      <c r="M6" s="95"/>
+      <c r="N6" s="93"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="91" t="s">
         <v>523</v>
       </c>
-      <c r="D6" s="94"/>
-      <c r="E6" s="94"/>
-      <c r="F6" s="94"/>
-      <c r="G6" s="94"/>
-      <c r="H6" s="94"/>
-      <c r="I6" s="93" t="n">
+      <c r="B7" s="96" t="n">
+        <v>365</v>
+      </c>
+      <c r="C7" s="91" t="s">
+        <v>525</v>
+      </c>
+      <c r="D7" s="97"/>
+      <c r="E7" s="97"/>
+      <c r="F7" s="97"/>
+      <c r="G7" s="97"/>
+      <c r="H7" s="97"/>
+      <c r="I7" s="96" t="n">
+        <v>180</v>
+      </c>
+      <c r="J7" s="96" t="n">
+        <v>210</v>
+      </c>
+      <c r="K7" s="97"/>
+      <c r="L7" s="97"/>
+      <c r="M7" s="97"/>
+      <c r="N7" s="91"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="98" t="s">
+        <v>523</v>
+      </c>
+      <c r="B8" s="99" t="n">
+        <v>1460</v>
+      </c>
+      <c r="C8" s="98" t="s">
+        <v>526</v>
+      </c>
+      <c r="D8" s="100"/>
+      <c r="E8" s="100"/>
+      <c r="F8" s="100"/>
+      <c r="G8" s="100"/>
+      <c r="H8" s="100"/>
+      <c r="I8" s="99" t="n">
+        <v>75</v>
+      </c>
+      <c r="J8" s="99" t="n">
+        <v>90</v>
+      </c>
+      <c r="K8" s="100"/>
+      <c r="L8" s="100"/>
+      <c r="M8" s="100"/>
+      <c r="N8" s="98"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="91" t="s">
+        <v>527</v>
+      </c>
+      <c r="B9" s="96" t="n">
+        <v>180</v>
+      </c>
+      <c r="C9" s="91" t="s">
+        <v>524</v>
+      </c>
+      <c r="D9" s="97"/>
+      <c r="E9" s="97"/>
+      <c r="F9" s="97"/>
+      <c r="G9" s="97"/>
+      <c r="H9" s="97"/>
+      <c r="I9" s="96" t="n">
         <v>280</v>
       </c>
-      <c r="J6" s="93" t="n">
+      <c r="J9" s="96" t="n">
         <v>330</v>
       </c>
-      <c r="K6" s="94"/>
-      <c r="L6" s="94"/>
-      <c r="M6" s="94"/>
-      <c r="N6" s="92"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="90" t="s">
-        <v>522</v>
-      </c>
-      <c r="B7" s="95" t="n">
+      <c r="K9" s="97"/>
+      <c r="L9" s="97"/>
+      <c r="M9" s="97"/>
+      <c r="N9" s="91"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="98" t="s">
+        <v>527</v>
+      </c>
+      <c r="B10" s="99" t="n">
         <v>365</v>
       </c>
-      <c r="C7" s="90" t="s">
+      <c r="C10" s="98" t="s">
+        <v>525</v>
+      </c>
+      <c r="D10" s="100"/>
+      <c r="E10" s="100"/>
+      <c r="F10" s="100"/>
+      <c r="G10" s="100"/>
+      <c r="H10" s="100"/>
+      <c r="I10" s="99" t="n">
+        <v>180</v>
+      </c>
+      <c r="J10" s="99" t="n">
+        <v>210</v>
+      </c>
+      <c r="K10" s="100"/>
+      <c r="L10" s="100"/>
+      <c r="M10" s="100"/>
+      <c r="N10" s="98"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="91" t="s">
+        <v>527</v>
+      </c>
+      <c r="B11" s="96" t="n">
+        <v>1460</v>
+      </c>
+      <c r="C11" s="91" t="s">
+        <v>526</v>
+      </c>
+      <c r="D11" s="97"/>
+      <c r="E11" s="97"/>
+      <c r="F11" s="97"/>
+      <c r="G11" s="97"/>
+      <c r="H11" s="97"/>
+      <c r="I11" s="96" t="n">
+        <v>75</v>
+      </c>
+      <c r="J11" s="96" t="n">
+        <v>90</v>
+      </c>
+      <c r="K11" s="97"/>
+      <c r="L11" s="97"/>
+      <c r="M11" s="97"/>
+      <c r="N11" s="91"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="98" t="s">
+        <v>523</v>
+      </c>
+      <c r="B12" s="99" t="n">
+        <v>65535</v>
+      </c>
+      <c r="C12" s="98" t="s">
+        <v>528</v>
+      </c>
+      <c r="D12" s="100"/>
+      <c r="E12" s="100"/>
+      <c r="F12" s="100"/>
+      <c r="G12" s="100"/>
+      <c r="H12" s="100"/>
+      <c r="I12" s="99" t="n">
+        <v>50</v>
+      </c>
+      <c r="J12" s="99" t="n">
+        <v>65</v>
+      </c>
+      <c r="K12" s="100"/>
+      <c r="L12" s="100"/>
+      <c r="M12" s="100"/>
+      <c r="N12" s="98"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="91" t="s">
+        <v>527</v>
+      </c>
+      <c r="B13" s="96" t="n">
+        <v>65535</v>
+      </c>
+      <c r="C13" s="91" t="s">
+        <v>528</v>
+      </c>
+      <c r="D13" s="97"/>
+      <c r="E13" s="97"/>
+      <c r="F13" s="97"/>
+      <c r="G13" s="97"/>
+      <c r="H13" s="97"/>
+      <c r="I13" s="96" t="n">
+        <v>50</v>
+      </c>
+      <c r="J13" s="96" t="n">
+        <v>65</v>
+      </c>
+      <c r="K13" s="97"/>
+      <c r="L13" s="97"/>
+      <c r="M13" s="97"/>
+      <c r="N13" s="91"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="98" t="s">
+        <v>529</v>
+      </c>
+      <c r="B14" s="99" t="n">
+        <v>180</v>
+      </c>
+      <c r="C14" s="98" t="s">
         <v>524</v>
       </c>
-      <c r="D7" s="96"/>
-      <c r="E7" s="96"/>
-      <c r="F7" s="96"/>
-      <c r="G7" s="96"/>
-      <c r="H7" s="96"/>
-      <c r="I7" s="95" t="n">
+      <c r="D14" s="100"/>
+      <c r="E14" s="100"/>
+      <c r="F14" s="100"/>
+      <c r="G14" s="100"/>
+      <c r="H14" s="100"/>
+      <c r="I14" s="99" t="n">
+        <v>280</v>
+      </c>
+      <c r="J14" s="99" t="n">
+        <v>330</v>
+      </c>
+      <c r="K14" s="100"/>
+      <c r="L14" s="100"/>
+      <c r="M14" s="100"/>
+      <c r="N14" s="98"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="91" t="s">
+        <v>529</v>
+      </c>
+      <c r="B15" s="96" t="n">
+        <v>365</v>
+      </c>
+      <c r="C15" s="91" t="s">
+        <v>525</v>
+      </c>
+      <c r="D15" s="97"/>
+      <c r="E15" s="97"/>
+      <c r="F15" s="97"/>
+      <c r="G15" s="97"/>
+      <c r="H15" s="97"/>
+      <c r="I15" s="96" t="n">
         <v>180</v>
       </c>
-      <c r="J7" s="95" t="n">
+      <c r="J15" s="96" t="n">
         <v>210</v>
       </c>
-      <c r="K7" s="96"/>
-      <c r="L7" s="96"/>
-      <c r="M7" s="96"/>
-      <c r="N7" s="90"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="97" t="s">
-        <v>522</v>
-      </c>
-      <c r="B8" s="98" t="n">
+      <c r="K15" s="97"/>
+      <c r="L15" s="97"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="91"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="98" t="s">
+        <v>529</v>
+      </c>
+      <c r="B16" s="99" t="n">
         <v>1460</v>
       </c>
-      <c r="C8" s="97" t="s">
-        <v>525</v>
-      </c>
-      <c r="D8" s="99"/>
-      <c r="E8" s="99"/>
-      <c r="F8" s="99"/>
-      <c r="G8" s="99"/>
-      <c r="H8" s="99"/>
-      <c r="I8" s="98" t="n">
+      <c r="C16" s="98" t="s">
+        <v>526</v>
+      </c>
+      <c r="D16" s="100"/>
+      <c r="E16" s="100"/>
+      <c r="F16" s="100"/>
+      <c r="G16" s="100"/>
+      <c r="H16" s="100"/>
+      <c r="I16" s="99" t="n">
         <v>75</v>
       </c>
-      <c r="J8" s="98" t="n">
+      <c r="J16" s="99" t="n">
         <v>90</v>
       </c>
-      <c r="K8" s="99"/>
-      <c r="L8" s="99"/>
-      <c r="M8" s="99"/>
-      <c r="N8" s="97"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="90" t="s">
-        <v>526</v>
-      </c>
-      <c r="B9" s="95" t="n">
-        <v>180</v>
-      </c>
-      <c r="C9" s="90" t="s">
+      <c r="K16" s="100"/>
+      <c r="L16" s="100"/>
+      <c r="M16" s="100"/>
+      <c r="N16" s="98"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="91" t="s">
+        <v>527</v>
+      </c>
+      <c r="B17" s="96" t="n">
+        <v>4380</v>
+      </c>
+      <c r="C17" s="91" t="s">
+        <v>528</v>
+      </c>
+      <c r="D17" s="97"/>
+      <c r="E17" s="97"/>
+      <c r="F17" s="97"/>
+      <c r="G17" s="97"/>
+      <c r="H17" s="97"/>
+      <c r="I17" s="96" t="n">
+        <v>50</v>
+      </c>
+      <c r="J17" s="97"/>
+      <c r="K17" s="97"/>
+      <c r="L17" s="97"/>
+      <c r="M17" s="97"/>
+      <c r="N17" s="91"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="98" t="s">
         <v>523</v>
       </c>
-      <c r="D9" s="96"/>
-      <c r="E9" s="96"/>
-      <c r="F9" s="96"/>
-      <c r="G9" s="96"/>
-      <c r="H9" s="96"/>
-      <c r="I9" s="95" t="n">
-        <v>280</v>
-      </c>
-      <c r="J9" s="95" t="n">
-        <v>330</v>
-      </c>
-      <c r="K9" s="96"/>
-      <c r="L9" s="96"/>
-      <c r="M9" s="96"/>
-      <c r="N9" s="90"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="97" t="s">
-        <v>526</v>
-      </c>
-      <c r="B10" s="98" t="n">
-        <v>365</v>
-      </c>
-      <c r="C10" s="97" t="s">
-        <v>524</v>
-      </c>
-      <c r="D10" s="99"/>
-      <c r="E10" s="99"/>
-      <c r="F10" s="99"/>
-      <c r="G10" s="99"/>
-      <c r="H10" s="99"/>
-      <c r="I10" s="98" t="n">
-        <v>180</v>
-      </c>
-      <c r="J10" s="98" t="n">
-        <v>210</v>
-      </c>
-      <c r="K10" s="99"/>
-      <c r="L10" s="99"/>
-      <c r="M10" s="99"/>
-      <c r="N10" s="97"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="90" t="s">
-        <v>526</v>
-      </c>
-      <c r="B11" s="95" t="n">
-        <v>1460</v>
-      </c>
-      <c r="C11" s="90" t="s">
-        <v>525</v>
-      </c>
-      <c r="D11" s="96"/>
-      <c r="E11" s="96"/>
-      <c r="F11" s="96"/>
-      <c r="G11" s="96"/>
-      <c r="H11" s="96"/>
-      <c r="I11" s="95" t="n">
-        <v>75</v>
-      </c>
-      <c r="J11" s="95" t="n">
-        <v>90</v>
-      </c>
-      <c r="K11" s="96"/>
-      <c r="L11" s="96"/>
-      <c r="M11" s="96"/>
-      <c r="N11" s="90"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="97" t="s">
-        <v>522</v>
-      </c>
-      <c r="B12" s="98" t="n">
-        <v>65535</v>
-      </c>
-      <c r="C12" s="97" t="s">
-        <v>527</v>
-      </c>
-      <c r="D12" s="99"/>
-      <c r="E12" s="99"/>
-      <c r="F12" s="99"/>
-      <c r="G12" s="99"/>
-      <c r="H12" s="99"/>
-      <c r="I12" s="98" t="n">
+      <c r="B18" s="99" t="n">
+        <v>4380</v>
+      </c>
+      <c r="C18" s="98" t="s">
+        <v>528</v>
+      </c>
+      <c r="D18" s="100"/>
+      <c r="E18" s="100"/>
+      <c r="F18" s="100"/>
+      <c r="G18" s="100"/>
+      <c r="H18" s="100"/>
+      <c r="I18" s="99" t="n">
         <v>50</v>
       </c>
-      <c r="J12" s="98" t="n">
-        <v>65</v>
-      </c>
-      <c r="K12" s="99"/>
-      <c r="L12" s="99"/>
-      <c r="M12" s="99"/>
-      <c r="N12" s="97"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="90" t="s">
-        <v>526</v>
-      </c>
-      <c r="B13" s="95" t="n">
-        <v>65535</v>
-      </c>
-      <c r="C13" s="90" t="s">
-        <v>527</v>
-      </c>
-      <c r="D13" s="96"/>
-      <c r="E13" s="96"/>
-      <c r="F13" s="96"/>
-      <c r="G13" s="96"/>
-      <c r="H13" s="96"/>
-      <c r="I13" s="95" t="n">
+      <c r="J18" s="100"/>
+      <c r="K18" s="100"/>
+      <c r="L18" s="100"/>
+      <c r="M18" s="100"/>
+      <c r="N18" s="98"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="91" t="s">
+        <v>529</v>
+      </c>
+      <c r="B19" s="96" t="n">
+        <v>4380</v>
+      </c>
+      <c r="C19" s="91" t="s">
+        <v>528</v>
+      </c>
+      <c r="D19" s="97"/>
+      <c r="E19" s="97"/>
+      <c r="F19" s="97"/>
+      <c r="G19" s="97"/>
+      <c r="H19" s="97"/>
+      <c r="I19" s="96" t="n">
         <v>50</v>
       </c>
-      <c r="J13" s="95" t="n">
-        <v>65</v>
-      </c>
-      <c r="K13" s="96"/>
-      <c r="L13" s="96"/>
-      <c r="M13" s="96"/>
-      <c r="N13" s="90"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="97" t="s">
-        <v>528</v>
-      </c>
-      <c r="B14" s="98" t="n">
-        <v>180</v>
-      </c>
-      <c r="C14" s="97" t="s">
-        <v>523</v>
-      </c>
-      <c r="D14" s="99"/>
-      <c r="E14" s="99"/>
-      <c r="F14" s="99"/>
-      <c r="G14" s="99"/>
-      <c r="H14" s="99"/>
-      <c r="I14" s="98" t="n">
-        <v>280</v>
-      </c>
-      <c r="J14" s="98" t="n">
-        <v>330</v>
-      </c>
-      <c r="K14" s="99"/>
-      <c r="L14" s="99"/>
-      <c r="M14" s="99"/>
-      <c r="N14" s="97"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="90" t="s">
-        <v>528</v>
-      </c>
-      <c r="B15" s="95" t="n">
-        <v>365</v>
-      </c>
-      <c r="C15" s="90" t="s">
-        <v>524</v>
-      </c>
-      <c r="D15" s="96"/>
-      <c r="E15" s="96"/>
-      <c r="F15" s="96"/>
-      <c r="G15" s="96"/>
-      <c r="H15" s="96"/>
-      <c r="I15" s="95" t="n">
-        <v>180</v>
-      </c>
-      <c r="J15" s="95" t="n">
-        <v>210</v>
-      </c>
-      <c r="K15" s="96"/>
-      <c r="L15" s="96"/>
-      <c r="M15" s="96"/>
-      <c r="N15" s="90"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="97" t="s">
-        <v>528</v>
-      </c>
-      <c r="B16" s="98" t="n">
-        <v>1460</v>
-      </c>
-      <c r="C16" s="97" t="s">
-        <v>525</v>
-      </c>
-      <c r="D16" s="99"/>
-      <c r="E16" s="99"/>
-      <c r="F16" s="99"/>
-      <c r="G16" s="99"/>
-      <c r="H16" s="99"/>
-      <c r="I16" s="98" t="n">
-        <v>75</v>
-      </c>
-      <c r="J16" s="98" t="n">
-        <v>90</v>
-      </c>
-      <c r="K16" s="99"/>
-      <c r="L16" s="99"/>
-      <c r="M16" s="99"/>
-      <c r="N16" s="97"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="90" t="s">
-        <v>526</v>
-      </c>
-      <c r="B17" s="95" t="n">
-        <v>4380</v>
-      </c>
-      <c r="C17" s="90" t="s">
-        <v>527</v>
-      </c>
-      <c r="D17" s="96"/>
-      <c r="E17" s="96"/>
-      <c r="F17" s="96"/>
-      <c r="G17" s="96"/>
-      <c r="H17" s="96"/>
-      <c r="I17" s="95" t="n">
-        <v>50</v>
-      </c>
-      <c r="J17" s="96"/>
-      <c r="K17" s="96"/>
-      <c r="L17" s="96"/>
-      <c r="M17" s="96"/>
-      <c r="N17" s="90"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="97" t="s">
-        <v>522</v>
-      </c>
-      <c r="B18" s="98" t="n">
-        <v>4380</v>
-      </c>
-      <c r="C18" s="97" t="s">
-        <v>527</v>
-      </c>
-      <c r="D18" s="99"/>
-      <c r="E18" s="99"/>
-      <c r="F18" s="99"/>
-      <c r="G18" s="99"/>
-      <c r="H18" s="99"/>
-      <c r="I18" s="98" t="n">
-        <v>50</v>
-      </c>
-      <c r="J18" s="99"/>
-      <c r="K18" s="99"/>
-      <c r="L18" s="99"/>
-      <c r="M18" s="99"/>
-      <c r="N18" s="97"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="90" t="s">
-        <v>528</v>
-      </c>
-      <c r="B19" s="95" t="n">
-        <v>4380</v>
-      </c>
-      <c r="C19" s="90" t="s">
-        <v>527</v>
-      </c>
-      <c r="D19" s="96"/>
-      <c r="E19" s="96"/>
-      <c r="F19" s="96"/>
-      <c r="G19" s="96"/>
-      <c r="H19" s="96"/>
-      <c r="I19" s="95" t="n">
-        <v>50</v>
-      </c>
-      <c r="J19" s="96"/>
-      <c r="K19" s="96"/>
-      <c r="L19" s="96"/>
-      <c r="M19" s="96"/>
-      <c r="N19" s="90"/>
+      <c r="J19" s="97"/>
+      <c r="K19" s="97"/>
+      <c r="L19" s="97"/>
+      <c r="M19" s="97"/>
+      <c r="N19" s="91"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
     </row>
   </sheetData>

</xml_diff>